<commit_message>
add FPGA project ，change interface controller BOM
</commit_message>
<xml_diff>
--- a/归档/V01/interface board/interface board1物料清单V01.xlsx
+++ b/归档/V01/interface board/interface board1物料清单V01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="312">
   <si>
     <t>CAP Aluminum Polymer electrolytic 50V 100U  SMD10.3x10.3x10</t>
   </si>
@@ -304,9 +304,6 @@
     <t>L1008</t>
   </si>
   <si>
-    <t>74437349047</t>
-  </si>
-  <si>
     <t>6.8uH</t>
   </si>
   <si>
@@ -542,9 +539,6 @@
   </si>
   <si>
     <t>SOP16-065-4_37</t>
-  </si>
-  <si>
-    <t>SN65HVD1792D</t>
   </si>
   <si>
     <t>ADM2582EBRWZ</t>
@@ -966,6 +960,10 @@
   </si>
   <si>
     <t>R208-R211</t>
+  </si>
+  <si>
+    <t>SN65HVD1792DR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1530,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:H72"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1547,7 +1545,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="26.25">
       <c r="A1" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1601,7 +1599,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1663,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>1</v>
@@ -1689,7 +1687,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>6</v>
@@ -1715,7 +1713,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
@@ -1741,7 +1739,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>15</v>
@@ -1767,7 +1765,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>18</v>
@@ -1790,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>39</v>
@@ -1816,10 +1814,10 @@
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>42</v>
@@ -1845,7 +1843,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>21</v>
@@ -1868,10 +1866,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>45</v>
@@ -1894,10 +1892,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>48</v>
@@ -1920,10 +1918,10 @@
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>50</v>
@@ -1946,7 +1944,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>52</v>
@@ -1972,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>55</v>
@@ -1998,10 +1996,10 @@
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>57</v>
@@ -2027,7 +2025,7 @@
         <v>23</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>24</v>
@@ -2050,10 +2048,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>59</v>
@@ -2076,10 +2074,10 @@
         <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>62</v>
@@ -2088,7 +2086,7 @@
         <v>63</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="27">
@@ -2102,10 +2100,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>64</v>
@@ -2128,10 +2126,10 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>67</v>
@@ -2154,10 +2152,10 @@
         <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>69</v>
@@ -2180,10 +2178,10 @@
         <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>71</v>
@@ -2206,10 +2204,10 @@
         <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>72</v>
@@ -2232,10 +2230,10 @@
         <v>8</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>75</v>
@@ -2258,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>78</v>
@@ -2284,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>82</v>
@@ -2304,25 +2302,25 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2336,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>86</v>
@@ -2362,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>89</v>
@@ -2374,7 +2372,7 @@
         <v>84</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2388,10 +2386,10 @@
         <v>2</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>91</v>
@@ -2400,7 +2398,7 @@
         <v>60</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2414,10 +2412,10 @@
         <v>2</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>93</v>
@@ -2433,26 +2431,26 @@
       <c r="A36" s="1">
         <v>31</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>96</v>
+      <c r="B36" s="1">
+        <v>74437349068</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="H36" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2460,25 +2458,25 @@
         <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2486,22 +2484,22 @@
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="1">
         <v>10</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>68</v>
@@ -2512,25 +2510,25 @@
         <v>34</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="1">
         <v>67</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="40.5">
@@ -2538,25 +2536,25 @@
         <v>35</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" s="1">
         <v>28</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2564,25 +2562,25 @@
         <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="G41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2590,25 +2588,25 @@
         <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="G42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2616,25 +2614,25 @@
         <v>38</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="G43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2642,25 +2640,25 @@
         <v>39</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="G44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2668,25 +2666,25 @@
         <v>40</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="G45" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2694,25 +2692,25 @@
         <v>41</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C46" s="1">
         <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2720,25 +2718,25 @@
         <v>42</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C47" s="1">
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G47" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2746,25 +2744,25 @@
         <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="1">
         <v>2</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2772,25 +2770,25 @@
         <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" s="1">
         <v>2</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G49" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2798,25 +2796,25 @@
         <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C50" s="1">
         <v>9</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G50" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2824,25 +2822,25 @@
         <v>46</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C51" s="1">
         <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="G51" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2850,25 +2848,25 @@
         <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C52" s="1">
         <v>7</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="40.5">
@@ -2876,25 +2874,25 @@
         <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" s="1">
         <v>29</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G53" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="27">
@@ -2902,25 +2900,25 @@
         <v>49</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C54" s="1">
         <v>16</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2928,25 +2926,25 @@
         <v>50</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="G55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="27">
@@ -2954,25 +2952,25 @@
         <v>51</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C56" s="1">
         <v>11</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G56" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="27">
@@ -2980,25 +2978,25 @@
         <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C57" s="1">
         <v>4</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3006,25 +3004,25 @@
         <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C58" s="1">
         <v>8</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="40.5">
@@ -3032,25 +3030,25 @@
         <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C59" s="1">
         <v>1</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E59" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G59" s="1" t="s">
+      <c r="H59" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3058,25 +3056,25 @@
         <v>55</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E60" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G60" s="1" t="s">
+      <c r="H60" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="27">
@@ -3084,25 +3082,25 @@
         <v>56</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C61" s="1">
         <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F61" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="27">
@@ -3110,25 +3108,25 @@
         <v>57</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C62" s="1">
         <v>3</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="27">
@@ -3136,25 +3134,25 @@
         <v>58</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C63" s="1">
         <v>1</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E63" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="H63" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3162,25 +3160,25 @@
         <v>59</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C64" s="1">
         <v>1</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G64" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="27">
@@ -3188,25 +3186,25 @@
         <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C65" s="1">
         <v>12</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F65" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H65" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="40.5">
@@ -3214,25 +3212,25 @@
         <v>61</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G66" s="1" t="s">
+      <c r="H66" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3240,25 +3238,25 @@
         <v>62</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>176</v>
+        <v>311</v>
       </c>
       <c r="C67" s="1">
         <v>11</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>176</v>
+        <v>311</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="27">
@@ -3266,25 +3264,25 @@
         <v>63</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C68" s="1">
         <v>8</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3292,25 +3290,25 @@
         <v>64</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C69" s="1">
         <v>4</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3318,25 +3316,25 @@
         <v>65</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C70" s="1">
         <v>2</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3344,25 +3342,25 @@
         <v>66</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C71" s="1">
         <v>2</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F71" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H71" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="27">
@@ -3370,25 +3368,25 @@
         <v>67</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E72" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="H72" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:8">

</xml_diff>